<commit_message>
cucumber related all jar files added in pom.xml
</commit_message>
<xml_diff>
--- a/testng_project/src/test/resources/TestData/OrangeHRM.xlsx
+++ b/testng_project/src/test/resources/TestData/OrangeHRM.xlsx
@@ -7,7 +7,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -375,8 +375,79 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="3" max="3" width="15.66406" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -388,9 +459,6 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -399,30 +467,21 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -432,62 +491,6 @@
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
keyword driven is completed
</commit_message>
<xml_diff>
--- a/testng_project/src/test/resources/TestData/OrangeHRM.xlsx
+++ b/testng_project/src/test/resources/TestData/OrangeHRM.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="0">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -49,6 +49,9 @@
     <t>Dashboard</t>
   </si>
   <si>
+    <t>Pass</t>
+  </si>
+  <si>
     <t>testCase02</t>
   </si>
   <si>
@@ -58,6 +61,9 @@
     <t>Invalid credentials</t>
   </si>
   <si>
+    <t>Fail</t>
+  </si>
+  <si>
     <t>testCase03</t>
   </si>
   <si>
@@ -67,10 +73,16 @@
     <t>testCase04</t>
   </si>
   <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Fail</t>
+    <t>testCase05</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>testCase06</t>
+  </si>
+  <si>
+    <t>testCase07</t>
   </si>
 </sst>
 </file>
@@ -408,23 +420,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="14.66406"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.44141"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="10.44141"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="10.44141"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="18.0"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.0"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.777344"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="18.0"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="18.0"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.777344"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="15.6">
+    <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -444,7 +456,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="15.6">
+    <row r="2" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -457,71 +469,101 @@
       <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s" s="1">
         <v>9</v>
       </c>
-      <c r="F2" t="s" s="0">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" s="1" customFormat="1" ht="15.6">
+      <c r="F2" t="s" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s" s="1">
         <v>9</v>
       </c>
-      <c r="F3" t="s" s="0">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" s="1" customFormat="1" ht="15.6">
+      <c r="F3" t="s" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" s="1" customFormat="1">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s" s="1">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" s="1" customFormat="1">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s" s="0">
+      <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" s="1" customFormat="1" ht="15.6">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="F5" t="s" s="0">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>